<commit_message>
add a baseclass to the minigame module
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Minigame.xlsx
+++ b/ConfigData/Xlsx/Minigame.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Id</t>
   </si>
@@ -92,6 +92,30 @@
   </si>
   <si>
     <t>智械危机</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>背景</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BgImage</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>t2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>t5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>t1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>t6</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -844,13 +868,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:D8" totalsRowShown="0">
-  <autoFilter ref="A3:D8"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:E8" totalsRowShown="0">
+  <autoFilter ref="A3:E8"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="3" name="Name"/>
     <tableColumn id="4" name="WindowId"/>
     <tableColumn id="5" name="IconPath"/>
+    <tableColumn id="2" name="BgImage"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1143,10 +1168,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1156,7 +1181,7 @@
     <col min="4" max="4" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1169,8 +1194,11 @@
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1183,8 +1211,11 @@
       <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1197,8 +1228,11 @@
       <c r="D3" t="s">
         <v>15</v>
       </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>17000001</v>
       </c>
@@ -1211,8 +1245,11 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>17000002</v>
       </c>
@@ -1226,7 +1263,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>17000003</v>
       </c>
@@ -1239,8 +1276,11 @@
       <c r="D6" t="s">
         <v>11</v>
       </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>17000004</v>
       </c>
@@ -1253,8 +1293,11 @@
       <c r="D7" t="s">
         <v>13</v>
       </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>17000005</v>
       </c>
@@ -1266,6 +1309,9 @@
       </c>
       <c r="D8" t="s">
         <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upload resource for russia block
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Minigame.xlsx
+++ b/ConfigData/Xlsx/Minigame.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Id</t>
   </si>
@@ -116,6 +116,14 @@
   </si>
   <si>
     <t>t6</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>俄罗斯块</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GameButton6</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -868,8 +876,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:E8" totalsRowShown="0">
-  <autoFilter ref="A3:E8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:E9" totalsRowShown="0">
+  <autoFilter ref="A3:E9"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="3" name="Name"/>
@@ -1168,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1314,6 +1322,20 @@
         <v>27</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>17000006</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9">
+        <v>1105</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
optimise the code of linkgame
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Minigame.xlsx
+++ b/ConfigData/Xlsx/Minigame.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Id</t>
   </si>
@@ -128,6 +128,10 @@
   </si>
   <si>
     <t>连连看</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GameButton7</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1115,7 +1119,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1283,7 +1287,7 @@
         <v>1106</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimise the mark rule show of minigame
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Minigame.xlsx
+++ b/ConfigData/Xlsx/Minigame.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>Id</t>
   </si>
@@ -132,13 +132,38 @@
   </si>
   <si>
     <t>GameButton7</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LvB</t>
+  </si>
+  <si>
+    <t>LvB</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LvA</t>
+  </si>
+  <si>
+    <t>LvA</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LvS</t>
+  </si>
+  <si>
+    <t>LvS</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -816,11 +841,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:E10" totalsRowShown="0">
-  <autoFilter ref="A3:E10"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:H10" totalsRowShown="0">
+  <autoFilter ref="A3:H10"/>
+  <tableColumns count="8">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="3" name="Name"/>
+    <tableColumn id="6" name="LvB"/>
+    <tableColumn id="7" name="LvA"/>
+    <tableColumn id="8" name="LvS"/>
     <tableColumn id="4" name="WindowId"/>
     <tableColumn id="5" name="IconPath"/>
     <tableColumn id="2" name="BgImage"/>
@@ -830,7 +858,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -905,6 +933,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -940,6 +985,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1116,20 +1178,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C5" sqref="C5:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.375" customWidth="1"/>
-    <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="3" max="5" width="6.625" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1137,16 +1200,25 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1154,16 +1226,25 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1171,16 +1252,25 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>17000001</v>
       </c>
@@ -1188,16 +1278,25 @@
         <v>18</v>
       </c>
       <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
+      </c>
+      <c r="F4">
         <v>1100</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>17000002</v>
       </c>
@@ -1205,13 +1304,22 @@
         <v>17</v>
       </c>
       <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>50</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
         <v>1101</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>17000003</v>
       </c>
@@ -1219,16 +1327,25 @@
         <v>21</v>
       </c>
       <c r="C6">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>50</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
         <v>1102</v>
       </c>
-      <c r="D6" t="s">
+      <c r="G6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" t="s">
+      <c r="H6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>17000004</v>
       </c>
@@ -1236,16 +1353,25 @@
         <v>19</v>
       </c>
       <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>50</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
         <v>1103</v>
       </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" t="s">
+      <c r="H7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>17000005</v>
       </c>
@@ -1253,16 +1379,25 @@
         <v>20</v>
       </c>
       <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
         <v>1104</v>
       </c>
-      <c r="D8" t="s">
+      <c r="G8" t="s">
         <v>14</v>
       </c>
-      <c r="E8" t="s">
+      <c r="H8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>17000006</v>
       </c>
@@ -1270,13 +1405,22 @@
         <v>28</v>
       </c>
       <c r="C9">
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <v>50</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
         <v>1105</v>
       </c>
-      <c r="D9" t="s">
+      <c r="G9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>17000007</v>
       </c>
@@ -1284,9 +1428,18 @@
         <v>30</v>
       </c>
       <c r="C10">
+        <v>30</v>
+      </c>
+      <c r="D10">
+        <v>50</v>
+      </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
+      <c r="F10">
         <v>1106</v>
       </c>
-      <c r="D10" t="s">
+      <c r="G10" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update minigame's mark level
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Minigame.xlsx
+++ b/ConfigData/Xlsx/Minigame.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1181,7 +1181,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:E10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1278,10 +1278,10 @@
         <v>18</v>
       </c>
       <c r="C4">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D4">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="E4">
         <v>100</v>
@@ -1304,10 +1304,10 @@
         <v>17</v>
       </c>
       <c r="C5">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D5">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="E5">
         <v>100</v>
@@ -1330,10 +1330,10 @@
         <v>30</v>
       </c>
       <c r="D6">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E6">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F6">
         <v>1102</v>
@@ -1353,13 +1353,13 @@
         <v>19</v>
       </c>
       <c r="C7">
-        <v>30</v>
+        <v>2000</v>
       </c>
       <c r="D7">
-        <v>50</v>
+        <v>3750</v>
       </c>
       <c r="E7">
-        <v>100</v>
+        <v>5000</v>
       </c>
       <c r="F7">
         <v>1103</v>
@@ -1385,7 +1385,7 @@
         <v>50</v>
       </c>
       <c r="E8">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="F8">
         <v>1104</v>
@@ -1405,13 +1405,13 @@
         <v>28</v>
       </c>
       <c r="C9">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="D9">
-        <v>50</v>
+        <v>1200</v>
       </c>
       <c r="E9">
-        <v>100</v>
+        <v>2000</v>
       </c>
       <c r="F9">
         <v>1105</v>
@@ -1428,13 +1428,13 @@
         <v>30</v>
       </c>
       <c r="C10">
-        <v>30</v>
+        <v>5000</v>
       </c>
       <c r="D10">
-        <v>50</v>
+        <v>8000</v>
       </c>
       <c r="E10">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="F10">
         <v>1106</v>

</xml_diff>

<commit_message>
finish the element rim game
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Minigame.xlsx
+++ b/ConfigData/Xlsx/Minigame.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Id</t>
   </si>
@@ -157,6 +157,18 @@
   </si>
   <si>
     <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>元素圈</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GameButton8</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>t8</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -841,8 +853,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:H10" totalsRowShown="0">
-  <autoFilter ref="A3:H10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:H11" totalsRowShown="0">
+  <autoFilter ref="A3:H11"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="3" name="Name"/>
@@ -1178,10 +1190,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1443,6 +1455,32 @@
         <v>31</v>
       </c>
     </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>17000008</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11">
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <v>21</v>
+      </c>
+      <c r="E11">
+        <v>27</v>
+      </c>
+      <c r="F11">
+        <v>1107</v>
+      </c>
+      <c r="G11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
a new vote game
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Minigame.xlsx
+++ b/ConfigData/Xlsx/Minigame.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>Id</t>
   </si>
@@ -181,6 +181,18 @@
   </si>
   <si>
     <t>t9</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>t10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GameButton10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>村长选举</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -865,8 +877,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:H12" totalsRowShown="0">
-  <autoFilter ref="A3:H12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:H13" totalsRowShown="0">
+  <autoFilter ref="A3:H13"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="3" name="Name"/>
@@ -1202,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1519,6 +1531,32 @@
         <v>44</v>
       </c>
     </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>17000010</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13">
+        <v>60</v>
+      </c>
+      <c r="D13">
+        <v>70</v>
+      </c>
+      <c r="E13">
+        <v>80</v>
+      </c>
+      <c r="F13">
+        <v>1109</v>
+      </c>
+      <c r="G13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add new game twentity one
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Minigame.xlsx
+++ b/ConfigData/Xlsx/Minigame.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>Id</t>
   </si>
@@ -193,6 +193,13 @@
   </si>
   <si>
     <t>村长选举</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>t11</t>
+  </si>
+  <si>
+    <t>二十一</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -877,8 +884,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:H13" totalsRowShown="0">
-  <autoFilter ref="A3:H13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:H14" totalsRowShown="0">
+  <autoFilter ref="A3:H14"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="3" name="Name"/>
@@ -1214,10 +1221,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1557,6 +1564,32 @@
         <v>45</v>
       </c>
     </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>17000011</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14">
+        <v>60</v>
+      </c>
+      <c r="D14">
+        <v>75</v>
+      </c>
+      <c r="E14">
+        <v>90</v>
+      </c>
+      <c r="F14">
+        <v>1110</v>
+      </c>
+      <c r="G14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finish the game 21
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Minigame.xlsx
+++ b/ConfigData/Xlsx/Minigame.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>Id</t>
   </si>
@@ -200,6 +200,10 @@
   </si>
   <si>
     <t>二十一</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GameButton11</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1223,8 +1227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1584,7 +1588,7 @@
         <v>1110</v>
       </c>
       <c r="G14" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H14" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
introduce new concept dungeon
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Minigame.xlsx
+++ b/ConfigData/Xlsx/Minigame.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mini" sheetId="1" r:id="rId1"/>
@@ -210,8 +210,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,6 +374,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -823,10 +832,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -888,17 +897,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:H14" totalsRowShown="0">
-  <autoFilter ref="A3:H14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:H14" totalsRowShown="0">
+  <autoFilter ref="A3:H14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Id"/>
-    <tableColumn id="3" name="Name"/>
-    <tableColumn id="6" name="LvB"/>
-    <tableColumn id="7" name="LvA"/>
-    <tableColumn id="8" name="LvS"/>
-    <tableColumn id="4" name="WindowId"/>
-    <tableColumn id="5" name="IconPath"/>
-    <tableColumn id="2" name="BgImage"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Name"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="LvB"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="LvA"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="LvS"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="WindowId"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="IconPath"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="BgImage"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1224,11 +1233,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1240,54 +1249,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>